<commit_message>
Added extra tests for speed saturation
</commit_message>
<xml_diff>
--- a/Admin/Testing vectors.xlsx
+++ b/Admin/Testing vectors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kathryn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kathryn/Desktop/CruiseControlEsterel/Admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E209E-7199-9148-B1D3-771CCA31793A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583853B9-EFDE-3647-9E5E-080AB3F2C53C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{221D3743-8EAB-0D44-8A37-B390D497FE26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="34">
   <si>
     <t xml:space="preserve">INPUTS </t>
   </si>
@@ -81,9 +81,6 @@
     <t>TEST 2 -Move from OFF to ON to OFF</t>
   </si>
   <si>
-    <t>TEST 6 - Moving from ON to STBY to DISABLE with resume button</t>
-  </si>
-  <si>
     <t>TEST 7 - Move from OFF to ON to DISABLE to ON</t>
   </si>
   <si>
@@ -114,7 +111,22 @@
     <t>TEST 8 -All buttons pressed (except off) in OFF state (Expect go to ON state and ignore all other buttons)</t>
   </si>
   <si>
-    <t>Should decrease</t>
+    <t>TEST 6a - Moving from ON to STBY to DISABLE with resume button</t>
+  </si>
+  <si>
+    <t>TEST 6b - Moving from ON to STBY to DISABLE with resume button</t>
+  </si>
+  <si>
+    <t>TEST 12 - QuickAccel button pressed and speed limited to speed max</t>
+  </si>
+  <si>
+    <t>TEST 12 - QuickDecel button pressed and speed limited to speed min</t>
+  </si>
+  <si>
+    <t>TEST 13 - On pressed with speed above speed max</t>
+  </si>
+  <si>
+    <t>TEST 13 - On pressed with speed below speed min</t>
   </si>
 </sst>
 </file>
@@ -482,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B49015B-7A33-6149-9C65-3EED520B6421}">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:AC120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,7 +523,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="Q1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -552,7 +564,7 @@
         <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2">
         <v>2</v>
@@ -596,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -640,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -1691,7 +1703,7 @@
         <v>20</v>
       </c>
       <c r="N37">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -1905,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -1948,7 +1960,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1959,7 +1971,7 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" t="b">
         <v>1</v>
       </c>
@@ -2035,7 +2047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" t="b">
         <v>0</v>
       </c>
@@ -2067,13 +2079,13 @@
         <v>35</v>
       </c>
       <c r="M52">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" t="b">
         <v>0</v>
       </c>
@@ -2111,9 +2123,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2134,8 +2146,30 @@
       <c r="N55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P55" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -2163,8 +2197,35 @@
       <c r="I57" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P57" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>3</v>
+      </c>
+      <c r="R57" t="s">
+        <v>4</v>
+      </c>
+      <c r="S57" t="s">
+        <v>5</v>
+      </c>
+      <c r="T57" t="s">
+        <v>6</v>
+      </c>
+      <c r="U57" t="s">
+        <v>7</v>
+      </c>
+      <c r="V57" t="s">
+        <v>8</v>
+      </c>
+      <c r="W57" t="s">
+        <v>9</v>
+      </c>
+      <c r="X57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" t="b">
         <v>1</v>
       </c>
@@ -2201,8 +2262,44 @@
       <c r="N58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P58" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="b">
+        <v>0</v>
+      </c>
+      <c r="R58" t="b">
+        <v>0</v>
+      </c>
+      <c r="S58" t="b">
+        <v>0</v>
+      </c>
+      <c r="T58" t="b">
+        <v>0</v>
+      </c>
+      <c r="U58" t="b">
+        <v>0</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58">
+        <v>0</v>
+      </c>
+      <c r="X58">
+        <v>35</v>
+      </c>
+      <c r="AA58">
+        <v>35</v>
+      </c>
+      <c r="AB58">
+        <v>0</v>
+      </c>
+      <c r="AC58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -2234,13 +2331,49 @@
         <v>35</v>
       </c>
       <c r="M59">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P59" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="b">
+        <v>0</v>
+      </c>
+      <c r="R59" t="b">
+        <v>0</v>
+      </c>
+      <c r="S59" t="b">
+        <v>0</v>
+      </c>
+      <c r="T59" t="b">
+        <v>0</v>
+      </c>
+      <c r="U59" t="b">
+        <v>0</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59">
+        <v>20</v>
+      </c>
+      <c r="X59">
+        <v>35</v>
+      </c>
+      <c r="AA59">
+        <v>35</v>
+      </c>
+      <c r="AB59">
+        <v>0</v>
+      </c>
+      <c r="AC59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -2260,27 +2393,63 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="L60">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N60">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P60" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="b">
+        <v>0</v>
+      </c>
+      <c r="R60" t="b">
+        <v>1</v>
+      </c>
+      <c r="S60" t="b">
+        <v>0</v>
+      </c>
+      <c r="T60" t="b">
+        <v>0</v>
+      </c>
+      <c r="U60" t="b">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>0</v>
+      </c>
+      <c r="X60">
+        <v>20</v>
+      </c>
+      <c r="AA60">
+        <v>20</v>
+      </c>
+      <c r="AB60">
+        <v>0</v>
+      </c>
+      <c r="AC60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2291,7 +2460,7 @@
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2571,7 @@
         <v>20</v>
       </c>
       <c r="N66">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -2445,7 +2614,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2577,7 +2746,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2701,7 +2870,7 @@
         <v>35</v>
       </c>
       <c r="M79">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N79">
         <v>3</v>
@@ -2733,10 +2902,10 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L80">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M80">
         <v>0</v>
@@ -2747,7 +2916,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -2906,10 +3075,10 @@
         <v>35</v>
       </c>
       <c r="L87">
-        <v>35</v>
+        <v>37.5</v>
       </c>
       <c r="M87">
-        <v>0</v>
+        <v>20.28</v>
       </c>
       <c r="N87">
         <v>2</v>
@@ -2917,7 +3086,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -3070,23 +3239,631 @@
         <v>0</v>
       </c>
       <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>35</v>
+      </c>
+      <c r="L94">
+        <v>32.5</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" t="s">
         <v>3</v>
       </c>
-      <c r="I94">
-        <v>35</v>
-      </c>
-      <c r="L94">
-        <v>35</v>
-      </c>
-      <c r="M94" t="s">
-        <v>29</v>
-      </c>
-      <c r="N94">
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" t="s">
+        <v>7</v>
+      </c>
+      <c r="G98" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" t="s">
+        <v>10</v>
+      </c>
+      <c r="L98" t="s">
+        <v>11</v>
+      </c>
+      <c r="M98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" t="b">
+        <v>1</v>
+      </c>
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>35</v>
+      </c>
+      <c r="L99">
+        <v>35</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" t="b">
+        <v>0</v>
+      </c>
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>149</v>
+      </c>
+      <c r="L100">
+        <v>149</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" t="b">
+        <v>0</v>
+      </c>
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>149</v>
+      </c>
+      <c r="L101">
+        <v>150</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E105" t="s">
+        <v>6</v>
+      </c>
+      <c r="F105" t="s">
+        <v>7</v>
+      </c>
+      <c r="G105" t="s">
+        <v>8</v>
+      </c>
+      <c r="H105" t="s">
+        <v>9</v>
+      </c>
+      <c r="I105" t="s">
+        <v>10</v>
+      </c>
+      <c r="L105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M105" t="s">
+        <v>12</v>
+      </c>
+      <c r="N105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" t="b">
+        <v>1</v>
+      </c>
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>35</v>
+      </c>
+      <c r="L106">
+        <v>35</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" t="b">
+        <v>0</v>
+      </c>
+      <c r="B107" t="b">
+        <v>0</v>
+      </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>31</v>
+      </c>
+      <c r="L107">
+        <v>31</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A108" t="b">
+        <v>0</v>
+      </c>
+      <c r="B108" t="b">
+        <v>0</v>
+      </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" t="b">
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>31</v>
+      </c>
+      <c r="L108">
+        <v>30</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+      <c r="G112" t="s">
+        <v>8</v>
+      </c>
+      <c r="H112" t="s">
+        <v>9</v>
+      </c>
+      <c r="I112" t="s">
+        <v>10</v>
+      </c>
+      <c r="L112" t="s">
+        <v>11</v>
+      </c>
+      <c r="M112" t="s">
+        <v>12</v>
+      </c>
+      <c r="N112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A113" t="b">
+        <v>0</v>
+      </c>
+      <c r="B113" t="b">
+        <v>0</v>
+      </c>
+      <c r="C113" t="b">
+        <v>0</v>
+      </c>
+      <c r="D113" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" t="b">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>160</v>
+      </c>
+      <c r="L113">
+        <v>160</v>
+      </c>
+      <c r="M113">
+        <v>0</v>
+      </c>
+      <c r="N113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A114" t="b">
+        <v>1</v>
+      </c>
+      <c r="B114" t="b">
+        <v>0</v>
+      </c>
+      <c r="C114" t="b">
+        <v>0</v>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" t="b">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>160</v>
+      </c>
+      <c r="L114">
+        <v>150</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" t="s">
+        <v>5</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" t="s">
+        <v>7</v>
+      </c>
+      <c r="G118" t="s">
+        <v>8</v>
+      </c>
+      <c r="H118" t="s">
+        <v>9</v>
+      </c>
+      <c r="I118" t="s">
+        <v>10</v>
+      </c>
+      <c r="L118" t="s">
+        <v>11</v>
+      </c>
+      <c r="M118" t="s">
+        <v>12</v>
+      </c>
+      <c r="N118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A119" t="b">
+        <v>0</v>
+      </c>
+      <c r="B119" t="b">
+        <v>0</v>
+      </c>
+      <c r="C119" t="b">
+        <v>0</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" t="b">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>20</v>
+      </c>
+      <c r="L119">
+        <v>20</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" t="b">
+        <v>1</v>
+      </c>
+      <c r="B120" t="b">
+        <v>0</v>
+      </c>
+      <c r="C120" t="b">
+        <v>0</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" t="b">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>20</v>
+      </c>
+      <c r="L120">
+        <v>30</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+      <c r="N120">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="A96:I96"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A116:I116"/>
     <mergeCell ref="A69:I69"/>
     <mergeCell ref="A75:I75"/>
     <mergeCell ref="A82:I82"/>
@@ -3094,12 +3871,13 @@
     <mergeCell ref="A48:I48"/>
     <mergeCell ref="A55:I55"/>
     <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="P55:X55"/>
     <mergeCell ref="A32:I32"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A41:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>